<commit_message>
feat: update Keychron VIA config to match current driver
</commit_message>
<xml_diff>
--- a/Settings/Keychron/Keys.xlsx
+++ b/Settings/Keychron/Keys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\markus\projects\wiki\Settings\Keychron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551B87D6-2C30-465E-BE90-7D9D0CC3E2B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49475C3-C5C5-48F3-A4CD-D01369D3BEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{19317676-018F-4702-80F9-F840FF8E359F}"/>
+    <workbookView xWindow="39180" yWindow="-3420" windowWidth="16290" windowHeight="15410" activeTab="1" xr2:uid="{19317676-018F-4702-80F9-F840FF8E359F}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
@@ -225,9 +225,6 @@
     <t>Roll</t>
   </si>
   <si>
-    <t>Break</t>
-  </si>
-  <si>
     <t>RGB Toggle</t>
   </si>
   <si>
@@ -253,6 +250,9 @@
   </si>
   <si>
     <t>Macro 0 (Win+Alt+K)</t>
+  </si>
+  <si>
+    <t>Break/Pause</t>
   </si>
 </sst>
 </file>
@@ -349,14 +349,10 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -394,7 +390,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -500,7 +496,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -642,7 +638,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -656,29 +652,29 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="1" max="1" width="14.81640625" customWidth="1"/>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="J2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="D5" t="s">
         <v>24</v>
       </c>
@@ -686,7 +682,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>0</v>
       </c>
@@ -703,7 +699,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -726,7 +722,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -746,7 +742,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="G9" t="s">
         <v>22</v>
       </c>
@@ -763,17 +759,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1740EC7-B063-4D2E-B0F9-7CEDAD2DC91E}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>32</v>
       </c>
@@ -784,7 +780,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -795,7 +791,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -806,7 +802,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -817,64 +813,64 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>31</v>
       </c>
       <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>39</v>
       </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
       <c r="B9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
feat: add CapsLock to Fn+Caps
</commit_message>
<xml_diff>
--- a/Settings/Keychron/Keys.xlsx
+++ b/Settings/Keychron/Keys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\markus\projects\wiki\Settings\Keychron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49475C3-C5C5-48F3-A4CD-D01369D3BEFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D4FB1E-9678-4BCF-8D44-6CF58B2E037E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="39180" yWindow="-3420" windowWidth="16290" windowHeight="15410" activeTab="1" xr2:uid="{19317676-018F-4702-80F9-F840FF8E359F}"/>
   </bookViews>
@@ -759,9 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1740EC7-B063-4D2E-B0F9-7CEDAD2DC91E}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -788,7 +786,7 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
feat: update Keychron config
</commit_message>
<xml_diff>
--- a/Settings/Keychron/Keys.xlsx
+++ b/Settings/Keychron/Keys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\markus\projects\wiki\Settings\Keychron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D4FB1E-9678-4BCF-8D44-6CF58B2E037E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EF08E8-16B3-49B2-8418-D33921F1D725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39180" yWindow="-3420" windowWidth="16290" windowHeight="15410" activeTab="1" xr2:uid="{19317676-018F-4702-80F9-F840FF8E359F}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{19317676-018F-4702-80F9-F840FF8E359F}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
   <si>
     <t>RGB Mode</t>
   </si>
@@ -253,6 +253,9 @@
   </si>
   <si>
     <t>Break/Pause</t>
+  </si>
+  <si>
+    <t>Macro 1 (Win+L)</t>
   </si>
 </sst>
 </file>
@@ -334,7 +337,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -350,9 +353,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -390,7 +393,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -496,7 +499,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -652,7 +655,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.81640625" customWidth="1"/>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
@@ -759,9 +762,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1740EC7-B063-4D2E-B0F9-7CEDAD2DC91E}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
@@ -871,7 +876,7 @@
         <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
feat: generalize AutoHotKey mappings
</commit_message>
<xml_diff>
--- a/Settings/Keychron/Keys.xlsx
+++ b/Settings/Keychron/Keys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\markus\projects\wiki\Settings\Keychron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56EF08E8-16B3-49B2-8418-D33921F1D725}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD921CA0-6C62-468A-B6B2-333BB0BDCF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{19317676-018F-4702-80F9-F840FF8E359F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{19317676-018F-4702-80F9-F840FF8E359F}"/>
   </bookViews>
   <sheets>
     <sheet name="Default" sheetId="1" r:id="rId1"/>
@@ -243,12 +243,6 @@
     <t>Calc</t>
   </si>
   <si>
-    <t>F14 (Slack/Franz)</t>
-  </si>
-  <si>
-    <t>F13 (KeePassXC)</t>
-  </si>
-  <si>
     <t>Macro 0 (Win+Alt+K)</t>
   </si>
   <si>
@@ -256,6 +250,12 @@
   </si>
   <si>
     <t>Macro 1 (Win+L)</t>
+  </si>
+  <si>
+    <t>F14 (KeePassXC)</t>
+  </si>
+  <si>
+    <t>F15 (Chat App)</t>
   </si>
 </sst>
 </file>
@@ -337,7 +337,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -353,9 +353,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -393,7 +393,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -499,7 +499,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -655,7 +655,7 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14.81640625" customWidth="1"/>
     <col min="2" max="2" width="2" bestFit="1" customWidth="1"/>
@@ -763,10 +763,10 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="20.54296875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
@@ -821,7 +821,7 @@
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
         <v>37</v>
@@ -835,7 +835,7 @@
         <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -854,7 +854,7 @@
         <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C10" t="s">
         <v>35</v>
@@ -865,7 +865,7 @@
         <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
@@ -876,7 +876,7 @@
         <v>42</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
feat: distribute Vim Arrows and Umlauts more convenient
</commit_message>
<xml_diff>
--- a/Settings/Keychron/Keys.xlsx
+++ b/Settings/Keychron/Keys.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-22.04\home\markus\projects\wiki\Settings\Keychron\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-24.04\home\markus\projects\wiki\Settings\Keychron\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD921CA0-6C62-468A-B6B2-333BB0BDCF7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB934CE-F6B2-491E-9B75-724A38A85B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" activeTab="1" xr2:uid="{19317676-018F-4702-80F9-F840FF8E359F}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="60">
   <si>
     <t>RGB Mode</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Esc</t>
   </si>
   <si>
-    <t>AltGr (RAlt)</t>
-  </si>
-  <si>
     <t>&lt;|&gt; (NUBS)</t>
   </si>
   <si>
@@ -256,13 +253,49 @@
   </si>
   <si>
     <t>F15 (Chat App)</t>
+  </si>
+  <si>
+    <t>F13 (Obsidian)</t>
+  </si>
+  <si>
+    <t>MO(3)</t>
+  </si>
+  <si>
+    <t>ß / -</t>
+  </si>
+  <si>
+    <t>F17</t>
+  </si>
+  <si>
+    <t>F18</t>
+  </si>
+  <si>
+    <t>F19</t>
+  </si>
+  <si>
+    <t>F20</t>
+  </si>
+  <si>
+    <t>F21</t>
+  </si>
+  <si>
+    <t>ü / [</t>
+  </si>
+  <si>
+    <t>ö / ;</t>
+  </si>
+  <si>
+    <t>ä / '</t>
+  </si>
+  <si>
+    <t>€ / 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -303,6 +336,12 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -760,10 +799,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1740EC7-B063-4D2E-B0F9-7CEDAD2DC91E}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -774,13 +813,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -796,93 +835,134 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>57</v>
+      </c>
+      <c r="C16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>